<commit_message>
test toegevoegd voor Join, Split en Paste
</commit_message>
<xml_diff>
--- a/Resultaten/Resultaten.xlsx
+++ b/Resultaten/Resultaten.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Grafiek1" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>size</t>
   </si>
@@ -37,6 +37,21 @@
   </si>
   <si>
     <t>Delete</t>
+  </si>
+  <si>
+    <t>Join</t>
+  </si>
+  <si>
+    <t>Split</t>
+  </si>
+  <si>
+    <t>Paste</t>
+  </si>
+  <si>
+    <t>left</t>
+  </si>
+  <si>
+    <t>right</t>
   </si>
 </sst>
 </file>
@@ -402,11 +417,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="377304704"/>
-        <c:axId val="377305880"/>
+        <c:axId val="276142496"/>
+        <c:axId val="277676848"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="377304704"/>
+        <c:axId val="276142496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -449,7 +464,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="377305880"/>
+        <c:crossAx val="277676848"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -457,7 +472,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="377305880"/>
+        <c:axId val="277676848"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -509,7 +524,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="377304704"/>
+        <c:crossAx val="276142496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1145,7 +1160,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="124" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="124" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1156,7 +1171,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9309919" cy="6083710"/>
+    <xdr:ext cx="9299677" cy="6073468"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Grafiek 1"/>
@@ -1442,15 +1457,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O24" sqref="O24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1463,8 +1478,23 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1478,13 +1508,28 @@
         <v>35</v>
       </c>
       <c r="E2">
-        <f>LOG(A2)</f>
+        <f t="shared" ref="E2:E9" si="0">LOG(A2)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>251</v>
+      </c>
+      <c r="K2">
+        <v>529</v>
+      </c>
+      <c r="L2">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
-        <f>+A2*10</f>
+        <f t="shared" ref="A3:A9" si="1">+A2*10</f>
         <v>10</v>
       </c>
       <c r="B3">
@@ -1497,13 +1542,30 @@
         <v>70</v>
       </c>
       <c r="E3">
-        <f>LOG(A3)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H3">
+        <f>IF(I3=1,H2*10,H2)</f>
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <f>IF(I2=10000,1,I2*10)</f>
+        <v>10</v>
+      </c>
+      <c r="J3">
+        <v>230</v>
+      </c>
+      <c r="K3">
+        <v>643</v>
+      </c>
+      <c r="L3">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4">
-        <f>+A3*10</f>
+        <f t="shared" si="1"/>
         <v>100</v>
       </c>
       <c r="B4">
@@ -1516,13 +1578,30 @@
         <v>105</v>
       </c>
       <c r="E4">
-        <f>LOG(A4)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H4">
+        <f t="shared" ref="H4:H16" si="2">IF(I4=1,H3*10,H3)</f>
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <f t="shared" ref="I4:I16" si="3">IF(I3=10000,1,I3*10)</f>
+        <v>100</v>
+      </c>
+      <c r="J4">
+        <v>129</v>
+      </c>
+      <c r="K4">
+        <v>352</v>
+      </c>
+      <c r="L4">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5">
-        <f>+A4*10</f>
+        <f t="shared" si="1"/>
         <v>1000</v>
       </c>
       <c r="B5">
@@ -1535,13 +1614,30 @@
         <v>145</v>
       </c>
       <c r="E5">
-        <f>LOG(A5)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H5">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="3"/>
+        <v>1000</v>
+      </c>
+      <c r="J5">
+        <v>182</v>
+      </c>
+      <c r="K5">
+        <v>358</v>
+      </c>
+      <c r="L5">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6">
-        <f>+A5*10</f>
+        <f t="shared" si="1"/>
         <v>10000</v>
       </c>
       <c r="B6">
@@ -1554,13 +1650,30 @@
         <v>290</v>
       </c>
       <c r="E6">
-        <f>LOG(A6)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H6">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="3"/>
+        <v>10000</v>
+      </c>
+      <c r="J6">
+        <v>564</v>
+      </c>
+      <c r="K6">
+        <v>442</v>
+      </c>
+      <c r="L6">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
-        <f>+A6*10</f>
+        <f t="shared" si="1"/>
         <v>100000</v>
       </c>
       <c r="B7">
@@ -1573,13 +1686,30 @@
         <v>630</v>
       </c>
       <c r="E7">
-        <f>LOG(A7)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H7">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <v>62</v>
+      </c>
+      <c r="K7">
+        <v>157</v>
+      </c>
+      <c r="L7">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8">
-        <f>+A7*10</f>
+        <f t="shared" si="1"/>
         <v>1000000</v>
       </c>
       <c r="B8">
@@ -1592,13 +1722,30 @@
         <v>1130</v>
       </c>
       <c r="E8">
-        <f>LOG(A8)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H8">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+      <c r="J8">
+        <v>74</v>
+      </c>
+      <c r="K8">
+        <v>272</v>
+      </c>
+      <c r="L8">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9">
-        <f>+A8*10</f>
+        <f t="shared" si="1"/>
         <v>10000000</v>
       </c>
       <c r="B9">
@@ -1611,8 +1758,348 @@
         <v>1400</v>
       </c>
       <c r="E9">
-        <f>LOG(A9)</f>
+        <f t="shared" si="0"/>
         <v>7</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
+      <c r="J9">
+        <v>109</v>
+      </c>
+      <c r="K9">
+        <v>327</v>
+      </c>
+      <c r="L9">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H10">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="3"/>
+        <v>1000</v>
+      </c>
+      <c r="J10">
+        <v>139</v>
+      </c>
+      <c r="K10">
+        <v>364</v>
+      </c>
+      <c r="L10">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H11">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="3"/>
+        <v>10000</v>
+      </c>
+      <c r="J11">
+        <v>579</v>
+      </c>
+      <c r="K11">
+        <v>528</v>
+      </c>
+      <c r="L11">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H12">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="J12">
+        <v>77</v>
+      </c>
+      <c r="K12">
+        <v>242</v>
+      </c>
+      <c r="L12">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H13">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+      <c r="J13">
+        <v>102</v>
+      </c>
+      <c r="K13">
+        <v>316</v>
+      </c>
+      <c r="L13">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H14">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
+      <c r="J14">
+        <v>124</v>
+      </c>
+      <c r="K14">
+        <v>389</v>
+      </c>
+      <c r="L14">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H15">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="3"/>
+        <v>1000</v>
+      </c>
+      <c r="J15">
+        <v>190</v>
+      </c>
+      <c r="K15">
+        <v>446</v>
+      </c>
+      <c r="L15">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H16">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="3"/>
+        <v>10000</v>
+      </c>
+      <c r="J16">
+        <v>678</v>
+      </c>
+      <c r="K16">
+        <v>606</v>
+      </c>
+      <c r="L16">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="17" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="H17">
+        <f t="shared" ref="H17:H24" si="4">IF(I17=1,H16*10,H16)</f>
+        <v>1000</v>
+      </c>
+      <c r="I17">
+        <f t="shared" ref="I17:I24" si="5">IF(I16=10000,1,I16*10)</f>
+        <v>1</v>
+      </c>
+      <c r="J17">
+        <v>104</v>
+      </c>
+      <c r="K17">
+        <v>365</v>
+      </c>
+      <c r="L17">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="18" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="H18">
+        <f t="shared" si="4"/>
+        <v>1000</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="J18">
+        <v>133</v>
+      </c>
+      <c r="K18">
+        <v>369</v>
+      </c>
+      <c r="L18">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="19" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="H19">
+        <f t="shared" si="4"/>
+        <v>1000</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="5"/>
+        <v>100</v>
+      </c>
+      <c r="J19">
+        <v>186</v>
+      </c>
+      <c r="K19">
+        <v>460</v>
+      </c>
+      <c r="L19">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="20" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="H20">
+        <f t="shared" si="4"/>
+        <v>1000</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="5"/>
+        <v>1000</v>
+      </c>
+      <c r="J20">
+        <v>218</v>
+      </c>
+      <c r="K20">
+        <v>568</v>
+      </c>
+      <c r="L20">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="21" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="H21">
+        <f t="shared" si="4"/>
+        <v>1000</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="5"/>
+        <v>10000</v>
+      </c>
+      <c r="J21">
+        <v>818</v>
+      </c>
+      <c r="K21">
+        <v>628</v>
+      </c>
+      <c r="L21">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="22" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="H22">
+        <f t="shared" si="4"/>
+        <v>10000</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="J22">
+        <v>170</v>
+      </c>
+      <c r="K22">
+        <v>432</v>
+      </c>
+      <c r="L22">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="23" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="H23">
+        <f t="shared" si="4"/>
+        <v>10000</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="J23">
+        <v>204</v>
+      </c>
+      <c r="K23">
+        <v>489</v>
+      </c>
+      <c r="L23">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="24" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="H24">
+        <f t="shared" si="4"/>
+        <v>10000</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="5"/>
+        <v>100</v>
+      </c>
+      <c r="J24">
+        <v>246</v>
+      </c>
+      <c r="K24">
+        <v>596</v>
+      </c>
+      <c r="L24">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="25" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="H25">
+        <f t="shared" ref="H25:H27" si="6">IF(I25=1,H24*10,H24)</f>
+        <v>10000</v>
+      </c>
+      <c r="I25">
+        <f t="shared" ref="I25:I27" si="7">IF(I24=10000,1,I24*10)</f>
+        <v>1000</v>
+      </c>
+      <c r="J25">
+        <v>380</v>
+      </c>
+      <c r="K25">
+        <v>672</v>
+      </c>
+      <c r="L25">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="26" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="H26">
+        <f t="shared" si="6"/>
+        <v>10000</v>
+      </c>
+      <c r="I26">
+        <f t="shared" si="7"/>
+        <v>10000</v>
+      </c>
+      <c r="J26">
+        <v>817</v>
+      </c>
+      <c r="K26">
+        <v>789</v>
+      </c>
+      <c r="L26">
+        <v>391</v>
       </c>
     </row>
   </sheetData>

</xml_diff>